<commit_message>
json funcionand valeu Gom3s
</commit_message>
<xml_diff>
--- a/src/metas.xlsx
+++ b/src/metas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guigu\OneDrive\Área de Trabalho\AureaBot\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0608A114-1F4B-45C4-89A1-DE6FF69B0606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73E1AE2-40E8-47E4-98E4-BD02BB27B821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{73FC0B26-8210-4731-AB5C-6D60C659D95E}"/>
   </bookViews>
@@ -48,18 +48,6 @@
     <t>Projetos</t>
   </si>
   <si>
-    <t>Ações compartilhadas</t>
-  </si>
-  <si>
-    <t>Membros que executam</t>
-  </si>
-  <si>
-    <t>Participação em eventos</t>
-  </si>
-  <si>
-    <t>Projetos de impacto</t>
-  </si>
-  <si>
     <t>53k</t>
   </si>
   <si>
@@ -67,6 +55,18 @@
   </si>
   <si>
     <t>NPS</t>
+  </si>
+  <si>
+    <t>Acoes_compartilhadas</t>
+  </si>
+  <si>
+    <t>Membros_que_executam</t>
+  </si>
+  <si>
+    <t>Projetos_de_impacto</t>
+  </si>
+  <si>
+    <t>Participacao_em_eventos</t>
   </si>
 </sst>
 </file>
@@ -421,7 +421,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,19 +442,19 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -462,7 +462,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>23</v>
@@ -488,7 +488,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>16</v>

</xml_diff>